<commit_message>
refactor: update 3D model
update 3D model
</commit_message>
<xml_diff>
--- a/pcb/OECU_BASE/OECU_BASE.xlsx
+++ b/pcb/OECU_BASE/OECU_BASE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.My_Tech_Studio\1.Project\MyOECU\pcb\OECU_BASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BBBD5C3-C3DF-4D89-BCC7-F1CC611DB30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17A2358-4CF5-4161-B8B1-AAF7AE2FB80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28500" yWindow="3396" windowWidth="21228" windowHeight="13188" xr2:uid="{40749F16-2507-4610-9C11-22D7A0B70302}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{40749F16-2507-4610-9C11-22D7A0B70302}"/>
   </bookViews>
   <sheets>
     <sheet name="OECU_BASE" sheetId="1" r:id="rId1"/>
@@ -526,21 +526,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,1096 +861,1098 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F235DB-BAA1-499C-A560-F75D75B97254}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.125" customWidth="1"/>
-    <col min="2" max="2" width="20.625" customWidth="1"/>
-    <col min="3" max="3" width="255.625" customWidth="1"/>
-    <col min="4" max="5" width="23.125" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="12.25" customWidth="1"/>
+    <col min="1" max="1" width="24.75" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24" style="5" customWidth="1"/>
+    <col min="3" max="3" width="104.5" style="5" customWidth="1"/>
+    <col min="4" max="5" width="26.625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.25" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="4">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <v>2</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>66</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
         <v>18</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>8</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="4">
         <v>2</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="4">
         <v>19</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="4">
         <v>2</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="4">
         <v>7</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="4">
         <v>7</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="G14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="4">
         <v>51</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2" t="s">
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2" t="s">
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2" t="s">
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="4">
         <v>3</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2" t="s">
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="4">
         <v>21</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="4">
         <v>3</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="4">
         <v>6</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="4">
         <v>2</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="1">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2" t="s">
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="4">
         <v>5</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="1">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="F31" s="4">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-      <c r="G32" s="2" t="s">
+      <c r="F32" s="4">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="1">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="F33" s="4">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F34" s="1">
-        <v>1</v>
-      </c>
-      <c r="G34" s="2" t="s">
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-      <c r="G35" s="2" t="s">
+      <c r="F35" s="4">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="4">
         <v>7</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="4">
         <v>2</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="1">
-        <v>1</v>
-      </c>
-      <c r="G38" s="2" t="s">
+      <c r="F38" s="4">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="1">
-        <v>1</v>
-      </c>
-      <c r="G39" s="2" t="s">
+      <c r="F39" s="4">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="4">
         <v>32</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="1">
-        <v>1</v>
-      </c>
-      <c r="G41" s="2" t="s">
+      <c r="F41" s="4">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="4">
         <v>14</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+    <row r="43" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="4">
         <v>36</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="4">
         <v>14</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F45" s="1">
-        <v>1</v>
-      </c>
-      <c r="G45" s="2" t="s">
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F46" s="1">
-        <v>1</v>
-      </c>
-      <c r="G46" s="2" t="s">
+      <c r="F46" s="4">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F47" s="1">
-        <v>1</v>
-      </c>
-      <c r="G47" s="2" t="s">
+      <c r="F47" s="4">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: fix a PCB bug
1.fix a PCB bug
</commit_message>
<xml_diff>
--- a/pcb/OECU_BASE/OECU_BASE.xlsx
+++ b/pcb/OECU_BASE/OECU_BASE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.My_Tech_Studio\1.Project\MyOECU\pcb\OECU_BASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64ED764A-3FD1-46AB-A2BB-A4FC10424D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8B1169-6082-4E8B-BF68-00480B253F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B9A022D8-4897-441A-ABB1-09236DF6A4F6}"/>
   </bookViews>
@@ -111,9 +111,6 @@
     <t>贴片电容 0402</t>
   </si>
   <si>
-    <t>C26, C39, C43, C57, C72, C86, C99, C116</t>
-  </si>
-  <si>
     <t>0402</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>104</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C6, C7, C9, C11, C12, C13, C15, C16, C17, C18, C19, C25, C29, C30, C31, C32, C35, C44, C45, C46, C47, C50, C51, C59, C60, C61, C62, C63, C66, C74, C75, C76, C77, C80, C83, C89, C90, C91, C92, C93, C96, C104, C105, C106, C107, C110, C113</t>
-  </si>
-  <si>
     <t>200K</t>
   </si>
   <si>
@@ -460,6 +454,14 @@
   </si>
   <si>
     <t>TF_card</t>
+  </si>
+  <si>
+    <t>C2, C3, C4, C5, C6, C7, C9, C11, C12, C13, C15, C16, C17, C18, C25, C29, C31, C32, C35, C44, C46, C47, C50, C51, C59, C61, C62, C63, C66, C74, C76, C77, C80, C83, C89, C91, C92, C93, C96, C104, C106, C107, C110, C113</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C19, C30, C45, C60, C75, C90, C105, C26, C39, C43, C57, C72, C86, C99, C116</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -868,7 +870,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1048,13 +1050,13 @@
         <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F8" s="1">
         <v>8</v>
@@ -1065,13 +1067,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -1088,13 +1090,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -1111,19 +1113,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -1134,19 +1136,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="1">
         <v>7</v>
@@ -1157,13 +1159,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>10</v>
@@ -1180,19 +1182,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="F14" s="1">
         <v>7</v>
@@ -1201,21 +1203,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>50</v>
+        <v>142</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F15" s="1">
         <v>51</v>
@@ -1226,13 +1228,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>10</v>
@@ -1249,19 +1251,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -1272,19 +1274,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -1295,19 +1297,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1318,19 +1320,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -1341,19 +1343,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F21" s="1">
         <v>3</v>
@@ -1364,19 +1366,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1387,13 +1389,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>10</v>
@@ -1410,19 +1412,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="E24" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
@@ -1433,19 +1435,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
@@ -1456,19 +1458,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="D26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="F26" s="1">
         <v>6</v>
@@ -1479,19 +1481,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
@@ -1502,19 +1504,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
@@ -1525,19 +1527,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
@@ -1548,19 +1550,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F30" s="1">
         <v>5</v>
@@ -1571,19 +1573,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -1594,19 +1596,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
@@ -1617,19 +1619,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
@@ -1640,19 +1642,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
@@ -1669,7 +1671,7 @@
         <v>8</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>10</v>
@@ -1681,41 +1683,41 @@
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="E36" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="F36" s="1">
         <v>7</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>10</v>
@@ -1727,7 +1729,7 @@
         <v>2</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1738,7 +1740,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>10</v>
@@ -1750,18 +1752,18 @@
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>10</v>
@@ -1773,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
@@ -1784,30 +1786,30 @@
         <v>26</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F40" s="1">
         <v>32</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>10</v>
@@ -1819,64 +1821,64 @@
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="E42" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="F42" s="1">
         <v>14</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F43" s="1">
         <v>36</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>10</v>
@@ -1888,76 +1890,76 @@
         <v>14</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="E45" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="E46" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="F46" s="1">
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="E47" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>